<commit_message>
Updated new keywords: updateJSONDataInResponseDetails(Response response, String jsonPath, String value) updateJSONDataWithFilePath(String payloadPath, String jsonPath, String value) updateJSONDataWithFileName(String jsonFileName, String jsonPath, String value) updateJSONData(String jsonString, String jsonPath, String value)
</commit_message>
<xml_diff>
--- a/src/main/resources/keywords/joq-web-sel-keywords.xlsx
+++ b/src/main/resources/keywords/joq-web-sel-keywords.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="794">
   <si>
     <t>Keywords</t>
   </si>
@@ -2384,6 +2384,30 @@
   </si>
   <si>
     <t>joq-web-sel-keywords</t>
+  </si>
+  <si>
+    <t>updateJSONDataInResponseDetails(Response response, String jsonPath, String value)</t>
+  </si>
+  <si>
+    <t>Method to update the JSON path node value in the API response and it will create the JSON file and store in /src/test/resources/APITesting/RequestPayload/</t>
+  </si>
+  <si>
+    <t>updateJSONDataWithFilePath(String payloadPath, String jsonPath, String value)</t>
+  </si>
+  <si>
+    <t>Method to update the JSON path value in the given JSON payload file</t>
+  </si>
+  <si>
+    <t>updateJSONDataWithFileName(String jsonFileName, String jsonPath, String value)</t>
+  </si>
+  <si>
+    <t>Method to update the JSON path value in the given JSON payload file. The payload file should be available in ./src/test/resources/APITesting/RequestPayload/ folder</t>
+  </si>
+  <si>
+    <t>updateJSONData(String jsonString, String jsonPath, String value)</t>
+  </si>
+  <si>
+    <t>Method to update the JSON path in the given JSON payload</t>
   </si>
 </sst>
 </file>
@@ -2732,7 +2756,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2840,6 +2864,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3888,7 +3918,7 @@
   <dimension ref="C2:D16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3899,10 +3929,10 @@
   <sheetData>
     <row r="2" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="39" t="s">
         <v>785</v>
       </c>
-      <c r="D3" s="38"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="21" t="s">
@@ -3957,7 +3987,7 @@
         <v>117</v>
       </c>
       <c r="D10" s="23">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -4006,7 +4036,7 @@
       </c>
       <c r="D16" s="20">
         <f>SUM(D4:D15)</f>
-        <v>372</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -9414,11 +9444,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9430,21 +9460,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="30" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="34">
+      <c r="A2" s="37">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -9453,12 +9483,12 @@
       <c r="C2" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="34">
+      <c r="A3" s="37">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -9467,12 +9497,12 @@
       <c r="C3" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="34">
+      <c r="A4" s="37">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -9481,12 +9511,12 @@
       <c r="C4" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="34">
+      <c r="A5" s="37">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -9495,12 +9525,12 @@
       <c r="C5" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="34">
+      <c r="A6" s="37">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -9509,189 +9539,245 @@
       <c r="C6" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="34">
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="37">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="34">
+        <v>786</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="37">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>142</v>
+        <v>788</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>789</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="34">
+      <c r="A9" s="37">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="34">
+        <v>790</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="37">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="34">
+        <v>792</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="37">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="34">
+        <v>139</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="37">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="34">
+        <v>141</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="37">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="34">
+        <v>143</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="37">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>154</v>
+        <v>145</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="34">
+      <c r="A15" s="37">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="34">
+        <v>147</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="37">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>165</v>
+        <v>149</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="34">
+      <c r="A17" s="37">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>402</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="34">
+        <v>151</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="37">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="34">
+        <v>153</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="37">
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="37">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="37">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="37">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="38">
+        <v>22</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" s="24" t="s">
         <v>406</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D23" s="25" t="s">
         <v>407</v>
       </c>
     </row>

</xml_diff>